<commit_message>
updated documentation for metaed project and generated artifacts
</commit_message>
<xml_diff>
--- a/docs/metaed-project/MetaEdOutput/Documentation/DataDictionary/SqlDataDictionary.xlsx
+++ b/docs/metaed-project/MetaEdOutput/Documentation/DataDictionary/SqlDataDictionary.xlsx
@@ -842,7 +842,7 @@
         <v>fizz</v>
       </c>
       <c r="C41" t="str">
-        <v>A student's submission for an assignment.</v>
+        <v>A user's submission of course work for an assignment.</v>
       </c>
     </row>
     <row r="42">
@@ -853,7 +853,7 @@
         <v>fizz</v>
       </c>
       <c r="C42" t="str">
-        <v>The type or types of submissions available for the assignment.</v>
+        <v>The type(s) of submissions available for the assignment.</v>
       </c>
     </row>
     <row r="43">
@@ -2892,7 +2892,7 @@
         <v>fizz</v>
       </c>
       <c r="C227" t="str">
-        <v>The grade received for a section enrollment.</v>
+        <v>A grade assigned to a user in a section.</v>
       </c>
     </row>
     <row r="228">
@@ -2903,7 +2903,7 @@
         <v>fizz</v>
       </c>
       <c r="C228" t="str">
-        <v>A course section defined in the source system.</v>
+        <v>An organized grouping of course content and users over a period of time for the purpose of providing instruction.</v>
       </c>
     </row>
     <row r="229">
@@ -6258,7 +6258,7 @@
         <v>fizz</v>
       </c>
       <c r="C530" t="str">
-        <v>A system user.</v>
+        <v>A person using the instructional system.</v>
       </c>
     </row>
     <row r="531">
@@ -6280,7 +6280,7 @@
         <v>fizz</v>
       </c>
       <c r="C532" t="str">
-        <v>A user's activity events within the source system.</v>
+        <v>An activity performed by a user within the instructional system.</v>
       </c>
     </row>
     <row r="533">
@@ -6291,7 +6291,7 @@
         <v>fizz</v>
       </c>
       <c r="C533" t="str">
-        <v>The association of a system user and course section. For a student, this would be a section enrollment. For a teacher, this would be a section assignment.</v>
+        <v>The association of a user and section. For a student, this would be a section enrollment. For a teacher, this would be a section assignment.</v>
       </c>
     </row>
     <row r="534">
@@ -10536,7 +10536,7 @@
         <v>DeletedAt</v>
       </c>
       <c r="D145" t="str">
-        <v>The date/time the record EntityStatus changed to deleted.</v>
+        <v>The datetime the record EntityStatus was changed to deleted.</v>
       </c>
       <c r="E145" t="str">
         <v>[DATETIME2](7)</v>
@@ -10565,7 +10565,7 @@
         <v>DueDateTime</v>
       </c>
       <c r="D146" t="str">
-        <v>The due date/time for the assignment.</v>
+        <v>The date and time the assignment is due.</v>
       </c>
       <c r="E146" t="str">
         <v>[DATETIME2](7)</v>
@@ -10594,7 +10594,7 @@
         <v>EndDateTime</v>
       </c>
       <c r="D147" t="str">
-        <v>The end date/time for the assignment. Students will no longer have access to the assignment after this date.</v>
+        <v>The end date and time for the assignment. Students will no longer have access to the assignment after this date.</v>
       </c>
       <c r="E147" t="str">
         <v>[DATETIME2](7)</v>
@@ -10768,7 +10768,7 @@
         <v>StartDateTime</v>
       </c>
       <c r="D153" t="str">
-        <v>The start date/time for the assignment. Students will have access to the assignment after this date.</v>
+        <v>The start date and time for the assignment. Students will have access to the assignment after this date.</v>
       </c>
       <c r="E153" t="str">
         <v>[DATETIME2](7)</v>
@@ -10855,7 +10855,7 @@
         <v>DeletedAt</v>
       </c>
       <c r="D156" t="str">
-        <v>The date/time the record EntityStatus changed to deleted.</v>
+        <v>The datetime the record EntityStatus was changed to deleted.</v>
       </c>
       <c r="E156" t="str">
         <v>[DATETIME2](7)</v>
@@ -11058,7 +11058,7 @@
         <v>Status</v>
       </c>
       <c r="D163" t="str">
-        <v>The status of the submission in relation to the late policy.</v>
+        <v>The status of the submission in relation to the late acceptance policy.</v>
       </c>
       <c r="E163" t="str">
         <v>[NVARCHAR](60)</v>
@@ -11087,7 +11087,7 @@
         <v>SubmissionDateTime</v>
       </c>
       <c r="D164" t="str">
-        <v>The date/time for the assignment submission.</v>
+        <v>The date and time of the assignment submission.</v>
       </c>
       <c r="E164" t="str">
         <v>[DATETIME2](7)</v>
@@ -11174,7 +11174,7 @@
         <v>SubmissionType</v>
       </c>
       <c r="D167" t="str">
-        <v>The type or types of submissions available for the assignment.</v>
+        <v>The type(s) of submissions available for the assignment.</v>
       </c>
       <c r="E167" t="str">
         <v>[NVARCHAR](60)</v>
@@ -31826,7 +31826,7 @@
         <v>DeletedAt</v>
       </c>
       <c r="D878" t="str">
-        <v>The date/time the record EntityStatus changed to deleted.</v>
+        <v>The datetime the record EntityStatus was changed to deleted.</v>
       </c>
       <c r="E878" t="str">
         <v>[DATETIME2](7)</v>
@@ -31884,7 +31884,7 @@
         <v>Grade</v>
       </c>
       <c r="D880" t="str">
-        <v>The user's letter or numeric grade for the section enrollment.</v>
+        <v>The user's letter or numeric grade for the section.</v>
       </c>
       <c r="E880" t="str">
         <v>[NVARCHAR](20)</v>
@@ -32116,7 +32116,7 @@
         <v>DeletedAt</v>
       </c>
       <c r="D888" t="str">
-        <v>The date/time the record EntityStatus changed to deleted.</v>
+        <v>The datetime the record EntityStatus was changed to deleted.</v>
       </c>
       <c r="E888" t="str">
         <v>[DATETIME2](7)</v>
@@ -80865,7 +80865,7 @@
         <v>DeletedAt</v>
       </c>
       <c r="D2564" t="str">
-        <v>The date/time the record EntityStatus changed to deleted.</v>
+        <v>The datetime the record EntityStatus was changed to deleted.</v>
       </c>
       <c r="E2564" t="str">
         <v>[DATETIME2](7)</v>
@@ -81155,7 +81155,7 @@
         <v>DeletedAt</v>
       </c>
       <c r="D2574" t="str">
-        <v>The date/time the record EntityStatus changed to deleted.</v>
+        <v>The datetime the record EntityStatus was changed to deleted.</v>
       </c>
       <c r="E2574" t="str">
         <v>[DATETIME2](7)</v>
@@ -81619,7 +81619,7 @@
         <v>DeletedAt</v>
       </c>
       <c r="D2590" t="str">
-        <v>The date/time the record EntityStatus changed to deleted.</v>
+        <v>The datetime the record EntityStatus was changed to deleted.</v>
       </c>
       <c r="E2590" t="str">
         <v>[DATETIME2](7)</v>
@@ -81822,7 +81822,7 @@
         <v>DeletedAt</v>
       </c>
       <c r="D2597" t="str">
-        <v>The date/time the record EntityStatus changed to deleted.</v>
+        <v>The datetime the record EntityStatus was changed to deleted.</v>
       </c>
       <c r="E2597" t="str">
         <v>[DATETIME2](7)</v>

</xml_diff>